<commit_message>
Update import team and fix check grade for course complete
</commit_message>
<xml_diff>
--- a/public/files/import_data.xlsx
+++ b/public/files/import_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\Microsoft.SkypeApp_kzf8qxf38zg5c!App\All (2)\EASIA_STAFFLIST_0806\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\elearning-easia\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55779902-9124-44D7-A609-9A060581C8F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76D2A4E-60C4-4347-A376-6E9FE7ABB1E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Staff List" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="100">
   <si>
     <t>Nữ</t>
   </si>
@@ -329,6 +329,18 @@
   </si>
   <si>
     <t>EA</t>
+  </si>
+  <si>
+    <t>Team code</t>
+  </si>
+  <si>
+    <t>Mã Team</t>
+  </si>
+  <si>
+    <t>TEAM1</t>
+  </si>
+  <si>
+    <t>TEAM2</t>
   </si>
 </sst>
 </file>
@@ -561,6 +573,27 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -570,9 +603,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -585,29 +615,11 @@
     <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -891,10 +903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF10"/>
+  <dimension ref="A1:AG10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,164 +918,168 @@
     <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="56.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="20.5703125" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="56.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="H1" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="K1" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="35" t="s">
+      <c r="L1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="L1" s="34" t="s">
+      <c r="M1" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="31" t="s">
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" s="31" t="s">
+      <c r="R1" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="30" t="s">
+      <c r="S1" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="31" t="s">
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="W1" s="32" t="s">
+      <c r="X1" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="X1" s="33" t="s">
+      <c r="Y1" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="33"/>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="26" t="s">
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="38"/>
+      <c r="AC1" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="AC1" s="26" t="s">
+      <c r="AD1" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="AD1" s="26" t="s">
+      <c r="AE1" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="AE1" s="23" t="s">
+      <c r="AF1" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="27" t="s">
+      <c r="AG1" s="33" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="7" t="s">
+    <row r="2" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="23"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="V2" s="31"/>
-      <c r="W2" s="32"/>
-      <c r="X2" s="7" t="s">
+      <c r="W2" s="23"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="AA2" s="6" t="s">
+      <c r="AB2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AB2" s="26"/>
-      <c r="AC2" s="26"/>
-      <c r="AD2" s="26"/>
+      <c r="AC2" s="24"/>
+      <c r="AD2" s="24"/>
       <c r="AE2" s="24"/>
-      <c r="AF2" s="28"/>
+      <c r="AF2" s="31"/>
+      <c r="AG2" s="34"/>
     </row>
-    <row r="3" spans="1:32" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>24</v>
       </c>
@@ -1088,72 +1104,75 @@
       <c r="H3" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="J3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="K3" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="L3" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="M3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="N3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="O3" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="20" t="s">
+      <c r="P3" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="Q3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="R3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="R3" s="7"/>
-      <c r="S3" s="6" t="s">
+      <c r="S3" s="7"/>
+      <c r="T3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="U3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="V3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="W3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="W3" s="10" t="s">
+      <c r="X3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="11" t="s">
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="Z3" s="11" t="s">
+      <c r="AA3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="AA3" s="11" t="s">
+      <c r="AB3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="AB3" s="8" t="s">
+      <c r="AC3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="AC3" s="8" t="s">
+      <c r="AD3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="AD3" s="8" t="s">
+      <c r="AE3" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="AE3" s="25"/>
-      <c r="AF3" s="29"/>
+      <c r="AF3" s="32"/>
+      <c r="AG3" s="35"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>0</v>
       </c>
@@ -1178,7 +1197,7 @@
       <c r="H4" s="3">
         <v>7</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <v>8</v>
       </c>
       <c r="J4" s="4">
@@ -1187,10 +1206,10 @@
       <c r="K4" s="4">
         <v>10</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="4">
         <v>11</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M4" s="5">
         <v>12</v>
       </c>
       <c r="N4" s="3">
@@ -1205,10 +1224,10 @@
       <c r="Q4" s="3">
         <v>16</v>
       </c>
-      <c r="R4" s="5">
+      <c r="R4" s="3">
         <v>17</v>
       </c>
-      <c r="S4" s="3">
+      <c r="S4" s="5">
         <v>18</v>
       </c>
       <c r="T4" s="3">
@@ -1223,10 +1242,10 @@
       <c r="W4" s="3">
         <v>22</v>
       </c>
-      <c r="X4" s="5">
+      <c r="X4" s="3">
         <v>23</v>
       </c>
-      <c r="Y4" s="3">
+      <c r="Y4" s="5">
         <v>24</v>
       </c>
       <c r="Z4" s="3">
@@ -1250,8 +1269,11 @@
       <c r="AF4" s="3">
         <v>31</v>
       </c>
+      <c r="AG4" s="3">
+        <v>32</v>
+      </c>
     </row>
-    <row r="5" spans="1:32" ht="48" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" ht="48" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>1</v>
       </c>
@@ -1276,78 +1298,81 @@
       <c r="H5" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="J5" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="K5" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="L5" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="L5" s="14">
+      <c r="M5" s="14">
         <v>30446</v>
       </c>
-      <c r="M5" s="12">
+      <c r="N5" s="12">
         <v>10</v>
       </c>
-      <c r="N5" s="12">
+      <c r="O5" s="12">
         <v>5</v>
       </c>
-      <c r="O5" s="12">
+      <c r="P5" s="12">
         <v>1983</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="Q5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Q5" s="2" t="s">
+      <c r="R5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="R5" s="15">
+      <c r="S5" s="15">
         <v>39580</v>
       </c>
-      <c r="S5" s="1">
+      <c r="T5" s="1">
         <v>12</v>
       </c>
-      <c r="T5" s="1">
+      <c r="U5" s="1">
         <v>5</v>
       </c>
-      <c r="U5" s="1">
+      <c r="V5" s="1">
         <v>2008</v>
       </c>
-      <c r="V5" s="12" t="s">
+      <c r="W5" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="W5" s="16" t="s">
+      <c r="X5" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="X5" s="15" t="s">
+      <c r="Y5" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="Y5" s="12">
+      <c r="Z5" s="12">
         <v>25</v>
       </c>
-      <c r="Z5" s="12">
+      <c r="AA5" s="12">
         <v>7</v>
       </c>
-      <c r="AA5" s="12">
+      <c r="AB5" s="12">
         <v>2003</v>
       </c>
-      <c r="AB5" s="12" t="s">
+      <c r="AC5" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="AC5" s="12" t="s">
+      <c r="AD5" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="AD5" s="12"/>
-      <c r="AE5" s="18" t="s">
+      <c r="AE5" s="12"/>
+      <c r="AF5" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="AF5" s="12" t="s">
+      <c r="AG5" s="12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:32" ht="48" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" ht="48" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -1372,78 +1397,81 @@
       <c r="H6" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="J6" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="K6" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="K6" s="13" t="s">
+      <c r="L6" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="L6" s="14">
+      <c r="M6" s="14">
         <v>31619</v>
       </c>
-      <c r="M6" s="12">
+      <c r="N6" s="12">
         <v>26</v>
       </c>
-      <c r="N6" s="12">
+      <c r="O6" s="12">
         <v>7</v>
       </c>
-      <c r="O6" s="12">
+      <c r="P6" s="12">
         <v>1986</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="Q6" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="R6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="R6" s="19">
+      <c r="S6" s="19">
         <v>40391</v>
       </c>
-      <c r="S6" s="1">
+      <c r="T6" s="1">
         <v>1</v>
       </c>
-      <c r="T6" s="1">
+      <c r="U6" s="1">
         <v>8</v>
       </c>
-      <c r="U6" s="1">
+      <c r="V6" s="1">
         <v>2010</v>
       </c>
-      <c r="V6" s="12" t="s">
+      <c r="W6" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="W6" s="16" t="s">
+      <c r="X6" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="X6" s="15" t="s">
+      <c r="Y6" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="Y6" s="12">
+      <c r="Z6" s="12">
         <v>4</v>
       </c>
-      <c r="Z6" s="12">
+      <c r="AA6" s="12">
         <v>3</v>
       </c>
-      <c r="AA6" s="12">
+      <c r="AB6" s="12">
         <v>2015</v>
       </c>
-      <c r="AB6" s="12" t="s">
+      <c r="AC6" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="AC6" s="12" t="s">
+      <c r="AD6" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="AD6" s="12"/>
-      <c r="AE6" s="17" t="s">
+      <c r="AE6" s="12"/>
+      <c r="AF6" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="AF6" s="12" t="s">
+      <c r="AG6" s="12" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:32" ht="48" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" ht="48" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -1468,119 +1496,123 @@
       <c r="H7" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="J7" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="K7" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="K7" s="13" t="s">
+      <c r="L7" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="L7" s="14">
+      <c r="M7" s="14">
         <v>31620</v>
       </c>
-      <c r="M7" s="12">
+      <c r="N7" s="12">
         <v>27</v>
       </c>
-      <c r="N7" s="12">
+      <c r="O7" s="12">
         <v>7</v>
       </c>
-      <c r="O7" s="12">
+      <c r="P7" s="12">
         <v>1986</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="Q7" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="R7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="R7" s="19">
+      <c r="S7" s="19">
         <v>40391</v>
       </c>
-      <c r="S7" s="1">
+      <c r="T7" s="1">
         <v>1</v>
       </c>
-      <c r="T7" s="1">
+      <c r="U7" s="1">
         <v>8</v>
       </c>
-      <c r="U7" s="1">
+      <c r="V7" s="1">
         <v>2010</v>
       </c>
-      <c r="V7" s="12" t="s">
+      <c r="W7" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="W7" s="16" t="s">
+      <c r="X7" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="X7" s="15" t="s">
+      <c r="Y7" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="Y7" s="12">
+      <c r="Z7" s="12">
         <v>4</v>
       </c>
-      <c r="Z7" s="12">
+      <c r="AA7" s="12">
         <v>3</v>
       </c>
-      <c r="AA7" s="12">
+      <c r="AB7" s="12">
         <v>2015</v>
       </c>
-      <c r="AB7" s="12" t="s">
+      <c r="AC7" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="AC7" s="12" t="s">
+      <c r="AD7" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="AD7" s="12"/>
-      <c r="AE7" s="17" t="s">
+      <c r="AE7" s="12"/>
+      <c r="AF7" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="AF7" s="12" t="s">
+      <c r="AG7" s="12" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:32" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:33" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
     </row>
-    <row r="10" spans="1:32" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:33" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="Q1:Q2"/>
+  <mergeCells count="24">
+    <mergeCell ref="AF1:AF3"/>
+    <mergeCell ref="AE1:AE2"/>
+    <mergeCell ref="AG1:AG3"/>
+    <mergeCell ref="AD1:AD2"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="AC1:AC2"/>
+    <mergeCell ref="Y1:AB1"/>
+    <mergeCell ref="R1:R2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="L1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="M1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="H1:H2"/>
-    <mergeCell ref="AE1:AE3"/>
-    <mergeCell ref="AD1:AD2"/>
-    <mergeCell ref="AF1:AF3"/>
-    <mergeCell ref="AC1:AC2"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="X1:AA1"/>
+    <mergeCell ref="I1:I2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="AE6" r:id="rId1" xr:uid="{17D5EC32-5C46-AD47-9FB5-52F61289063A}"/>
-    <hyperlink ref="AE5" r:id="rId2" xr:uid="{7FC0A234-CA60-5049-8E36-12DA086286D9}"/>
-    <hyperlink ref="AE7" r:id="rId3" xr:uid="{11841F35-A7C4-4374-B571-4371FB9F9042}"/>
+    <hyperlink ref="AF6" r:id="rId1" xr:uid="{17D5EC32-5C46-AD47-9FB5-52F61289063A}"/>
+    <hyperlink ref="AF5" r:id="rId2" xr:uid="{7FC0A234-CA60-5049-8E36-12DA086286D9}"/>
+    <hyperlink ref="AF7" r:id="rId3" xr:uid="{11841F35-A7C4-4374-B571-4371FB9F9042}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
[TMS][FIX] Start working date import excel, description column deparment code and organization code
</commit_message>
<xml_diff>
--- a/public/files/import_data.xlsx
+++ b/public/files/import_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\elearning-easia\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76D2A4E-60C4-4347-A376-6E9FE7ABB1E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5CC775-46DD-4D6E-8E00-CB573BD76225}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -265,9 +265,6 @@
     <t>easia.vdm</t>
   </si>
   <si>
-    <t>Mã phòng / Bộ phận</t>
-  </si>
-  <si>
     <t>Department code</t>
   </si>
   <si>
@@ -325,9 +322,6 @@
     <t>Organization code</t>
   </si>
   <si>
-    <t>Mã tổ chức</t>
-  </si>
-  <si>
     <t>EA</t>
   </si>
   <si>
@@ -341,6 +335,36 @@
   </si>
   <si>
     <t>TEAM2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mã phòng / Bộ phận 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(SLS / CON / ACC / ...)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mã tổ chức
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(EA / EV / AV /  BG / ...)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -573,11 +597,38 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -593,33 +644,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -906,7 +930,7 @@
   <dimension ref="A1:AG10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,8 +941,9 @@
     <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="8" max="8" width="25.28515625" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" customWidth="1"/>
     <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
@@ -946,107 +971,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="H1" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="I1" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="J1" s="24" t="s">
+      <c r="G1" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="L1" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="M1" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="23" t="s">
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="R1" s="23" t="s">
+      <c r="R1" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="S1" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="36"/>
-      <c r="U1" s="36"/>
-      <c r="V1" s="36"/>
-      <c r="W1" s="23" t="s">
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="X1" s="37" t="s">
+      <c r="X1" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" s="38" t="s">
+      <c r="Y1" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="Z1" s="38"/>
-      <c r="AA1" s="38"/>
-      <c r="AB1" s="38"/>
-      <c r="AC1" s="24" t="s">
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" s="24" t="s">
+      <c r="AD1" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="AE1" s="24" t="s">
+      <c r="AE1" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="AF1" s="30" t="s">
+      <c r="AF1" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="AG1" s="33" t="s">
+      <c r="AG1" s="27" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
       <c r="S2" s="7" t="s">
         <v>17</v>
       </c>
@@ -1059,8 +1084,8 @@
       <c r="V2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="W2" s="23"/>
-      <c r="X2" s="37"/>
+      <c r="W2" s="31"/>
+      <c r="X2" s="32"/>
       <c r="Y2" s="7" t="s">
         <v>17</v>
       </c>
@@ -1073,13 +1098,13 @@
       <c r="AB2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AC2" s="24"/>
-      <c r="AD2" s="24"/>
-      <c r="AE2" s="24"/>
-      <c r="AF2" s="31"/>
-      <c r="AG2" s="34"/>
+      <c r="AC2" s="26"/>
+      <c r="AD2" s="26"/>
+      <c r="AE2" s="26"/>
+      <c r="AF2" s="24"/>
+      <c r="AG2" s="28"/>
     </row>
-    <row r="3" spans="1:33" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>24</v>
       </c>
@@ -1098,14 +1123,14 @@
       <c r="F3" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>94</v>
+      <c r="G3" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>99</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J3" s="21" t="s">
         <v>18</v>
@@ -1169,8 +1194,8 @@
       <c r="AE3" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="AF3" s="32"/>
-      <c r="AG3" s="35"/>
+      <c r="AF3" s="25"/>
+      <c r="AG3" s="29"/>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
@@ -1293,22 +1318,22 @@
         <v>55</v>
       </c>
       <c r="G5" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="K5" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="K5" s="13" t="s">
+      <c r="L5" s="13" t="s">
         <v>77</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>78</v>
       </c>
       <c r="M5" s="14">
         <v>30446</v>
@@ -1392,22 +1417,22 @@
         <v>55</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J6" s="13" t="s">
         <v>56</v>
       </c>
       <c r="K6" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="L6" s="13" t="s">
         <v>77</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>78</v>
       </c>
       <c r="M6" s="14">
         <v>31619</v>
@@ -1476,37 +1501,37 @@
         <v>2</v>
       </c>
       <c r="B7" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="D7" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="E7" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="F7" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="G7" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="H7" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="J7" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="G7" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>86</v>
-      </c>
       <c r="K7" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="L7" s="13" t="s">
         <v>77</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>78</v>
       </c>
       <c r="M7" s="14">
         <v>31620</v>
@@ -1521,7 +1546,7 @@
         <v>1986</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="R7" s="2" t="s">
         <v>1</v>
@@ -1539,10 +1564,10 @@
         <v>2010</v>
       </c>
       <c r="W7" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="X7" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Y7" s="15" t="s">
         <v>70</v>
@@ -1557,17 +1582,17 @@
         <v>2015</v>
       </c>
       <c r="AC7" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AD7" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AE7" s="12"/>
       <c r="AF7" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="AG7" s="12" t="s">
         <v>90</v>
-      </c>
-      <c r="AG7" s="12" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:33" ht="26.25" x14ac:dyDescent="0.4">
@@ -1584,15 +1609,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="AF1:AF3"/>
-    <mergeCell ref="AE1:AE2"/>
-    <mergeCell ref="AG1:AG3"/>
-    <mergeCell ref="AD1:AD2"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="AC1:AC2"/>
-    <mergeCell ref="Y1:AB1"/>
     <mergeCell ref="R1:R2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C1:C2"/>
@@ -1608,6 +1624,15 @@
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
+    <mergeCell ref="AF1:AF3"/>
+    <mergeCell ref="AE1:AE2"/>
+    <mergeCell ref="AG1:AG3"/>
+    <mergeCell ref="AD1:AD2"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="AC1:AC2"/>
+    <mergeCell ref="Y1:AB1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="AF6" r:id="rId1" xr:uid="{17D5EC32-5C46-AD47-9FB5-52F61289063A}"/>

</xml_diff>

<commit_message>
[TMS][Update] Add line manager to db and import user function
</commit_message>
<xml_diff>
--- a/public/files/import_data.xlsx
+++ b/public/files/import_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\elearning-easia\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5CC775-46DD-4D6E-8E00-CB573BD76225}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B711BF4-7EC0-44B2-92AD-084C755F0B4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="101">
   <si>
     <t>Nữ</t>
   </si>
@@ -365,6 +365,9 @@
       </rPr>
       <t>(EA / EV / AV /  BG / ...)</t>
     </r>
+  </si>
+  <si>
+    <t>Line Manager</t>
   </si>
 </sst>
 </file>
@@ -597,6 +600,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -608,15 +620,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -927,10 +930,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG10"/>
+  <dimension ref="A1:AH10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH6" sqref="AH6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,22 +971,23 @@
     <col min="31" max="31" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="16" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="32.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>43</v>
       </c>
       <c r="B1" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="29" t="s">
         <v>39</v>
       </c>
       <c r="F1" s="31" t="s">
@@ -998,7 +1002,7 @@
       <c r="I1" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="29" t="s">
         <v>37</v>
       </c>
       <c r="K1" s="35" t="s">
@@ -1037,33 +1041,36 @@
       <c r="Z1" s="33"/>
       <c r="AA1" s="33"/>
       <c r="AB1" s="33"/>
-      <c r="AC1" s="26" t="s">
+      <c r="AC1" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" s="26" t="s">
+      <c r="AD1" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="AE1" s="26" t="s">
+      <c r="AE1" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="AF1" s="23" t="s">
+      <c r="AF1" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="AG1" s="27" t="s">
+      <c r="AG1" s="23" t="s">
         <v>48</v>
       </c>
+      <c r="AH1" s="23" t="s">
+        <v>100</v>
+      </c>
     </row>
-    <row r="2" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="31"/>
       <c r="B2" s="38"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
       <c r="F2" s="31"/>
       <c r="G2" s="38"/>
       <c r="H2" s="38"/>
       <c r="I2" s="38"/>
-      <c r="J2" s="26"/>
+      <c r="J2" s="29"/>
       <c r="K2" s="36"/>
       <c r="L2" s="36"/>
       <c r="M2" s="34"/>
@@ -1098,13 +1105,14 @@
       <c r="AB2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AC2" s="26"/>
-      <c r="AD2" s="26"/>
-      <c r="AE2" s="26"/>
-      <c r="AF2" s="24"/>
-      <c r="AG2" s="28"/>
+      <c r="AC2" s="29"/>
+      <c r="AD2" s="29"/>
+      <c r="AE2" s="29"/>
+      <c r="AF2" s="27"/>
+      <c r="AG2" s="24"/>
+      <c r="AH2" s="24"/>
     </row>
-    <row r="3" spans="1:33" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>24</v>
       </c>
@@ -1194,10 +1202,11 @@
       <c r="AE3" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="AF3" s="25"/>
-      <c r="AG3" s="29"/>
+      <c r="AF3" s="28"/>
+      <c r="AG3" s="25"/>
+      <c r="AH3" s="25"/>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>0</v>
       </c>
@@ -1297,8 +1306,11 @@
       <c r="AG4" s="3">
         <v>32</v>
       </c>
+      <c r="AH4" s="3">
+        <v>33</v>
+      </c>
     </row>
-    <row r="5" spans="1:33" ht="48" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" ht="48" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>1</v>
       </c>
@@ -1396,8 +1408,9 @@
       <c r="AG5" s="12" t="s">
         <v>63</v>
       </c>
+      <c r="AH5" s="17"/>
     </row>
-    <row r="6" spans="1:33" ht="48" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:34" ht="48" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -1495,8 +1508,11 @@
       <c r="AG6" s="12" t="s">
         <v>73</v>
       </c>
+      <c r="AH6" s="18" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="7" spans="1:33" ht="48" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:34" ht="48" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -1594,21 +1610,24 @@
       <c r="AG7" s="12" t="s">
         <v>90</v>
       </c>
+      <c r="AH7" s="18" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="9" spans="1:33" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:34" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
     </row>
-    <row r="10" spans="1:33" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:34" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="25">
     <mergeCell ref="R1:R2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C1:C2"/>
@@ -1624,22 +1643,25 @@
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
-    <mergeCell ref="AF1:AF3"/>
-    <mergeCell ref="AE1:AE2"/>
-    <mergeCell ref="AG1:AG3"/>
-    <mergeCell ref="AD1:AD2"/>
     <mergeCell ref="S1:V1"/>
     <mergeCell ref="W1:W2"/>
     <mergeCell ref="X1:X2"/>
     <mergeCell ref="AC1:AC2"/>
     <mergeCell ref="Y1:AB1"/>
+    <mergeCell ref="AH1:AH3"/>
+    <mergeCell ref="AG1:AG3"/>
+    <mergeCell ref="AF1:AF3"/>
+    <mergeCell ref="AE1:AE2"/>
+    <mergeCell ref="AD1:AD2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="AF6" r:id="rId1" xr:uid="{17D5EC32-5C46-AD47-9FB5-52F61289063A}"/>
     <hyperlink ref="AF5" r:id="rId2" xr:uid="{7FC0A234-CA60-5049-8E36-12DA086286D9}"/>
     <hyperlink ref="AF7" r:id="rId3" xr:uid="{11841F35-A7C4-4374-B571-4371FB9F9042}"/>
+    <hyperlink ref="AH6" r:id="rId4" xr:uid="{6A597F78-6AE2-4047-8608-302DE6000859}"/>
+    <hyperlink ref="AH7" r:id="rId5" xr:uid="{E13CBC06-8837-4264-8BC0-3D2BFC682668}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[TMS][Update] Optional roles for organization management, import data
</commit_message>
<xml_diff>
--- a/public/files/import_data.xlsx
+++ b/public/files/import_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\elearning-easia\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B711BF4-7EC0-44B2-92AD-084C755F0B4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4EF30E5-E2E3-455D-80E8-44215B22F96A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="118">
   <si>
     <t>Nữ</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>dd/mm/year</t>
-  </si>
-  <si>
-    <t>Vị trí/chức danh</t>
   </si>
   <si>
     <t>Phòng/Bộ phận</t>
@@ -368,6 +365,60 @@
   </si>
   <si>
     <t>Line Manager</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Chức danh</t>
+  </si>
+  <si>
+    <t>Vị trí</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Senior Executive</t>
+  </si>
+  <si>
+    <t>NGUYỄN VĂN B</t>
+  </si>
+  <si>
+    <t>NGUYỄN VĂN C</t>
+  </si>
+  <si>
+    <t>Leader</t>
+  </si>
+  <si>
+    <t>Contacting Leader - French Speaking Market - FIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Executive</t>
+  </si>
+  <si>
+    <t>Contacting Junior Executive - French Speaking Market - FIT</t>
+  </si>
+  <si>
+    <t>Junior Executive</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>nguyenvanb@easia-travel.com</t>
+  </si>
+  <si>
+    <t>nguyenvanc@easia-travel.com</t>
+  </si>
+  <si>
+    <t>easia.contacting2</t>
+  </si>
+  <si>
+    <t>easia.contacting3</t>
   </si>
 </sst>
 </file>
@@ -534,7 +585,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -600,6 +651,36 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -618,35 +699,11 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -930,10 +987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH10"/>
+  <dimension ref="A1:AI10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH6" sqref="AH6"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AG12" sqref="AG12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,142 +1005,144 @@
     <col min="8" max="8" width="25.28515625" customWidth="1"/>
     <col min="9" max="9" width="20.5703125" customWidth="1"/>
     <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="56.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="56.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="32.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="37" t="s">
+    <row r="1" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="C1" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="D1" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="E1" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="H1" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="I1" s="37" t="s">
-        <v>94</v>
-      </c>
-      <c r="J1" s="29" t="s">
+      <c r="F1" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="L1" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="M1" s="34" t="s">
+      <c r="G1" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="K1" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="31" t="s">
+      <c r="L1" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="R1" s="31" t="s">
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="S1" s="30" t="s">
+      <c r="S1" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="30"/>
+      <c r="T1" s="30" t="s">
+        <v>32</v>
+      </c>
       <c r="U1" s="30"/>
       <c r="V1" s="30"/>
-      <c r="W1" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="X1" s="32" t="s">
+      <c r="W1" s="30"/>
+      <c r="X1" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" s="33" t="s">
+      <c r="Y1" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="Z1" s="33"/>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="33"/>
-      <c r="AC1" s="29" t="s">
+      <c r="Z1" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="AE1" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF1" s="26" t="s">
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="AG1" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="AH1" s="23" t="s">
-        <v>100</v>
+      <c r="AE1" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF1" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG1" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH1" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI1" s="33" t="s">
+        <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="7" t="s">
+    <row r="2" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="23"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="U2" s="6" t="s">
         <v>26</v>
@@ -1091,13 +1150,13 @@
       <c r="V2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="W2" s="31"/>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="7" t="s">
+      <c r="W2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="X2" s="23"/>
+      <c r="Y2" s="31"/>
+      <c r="Z2" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="Z2" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="AA2" s="6" t="s">
         <v>26</v>
@@ -1105,108 +1164,114 @@
       <c r="AB2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AC2" s="29"/>
-      <c r="AD2" s="29"/>
-      <c r="AE2" s="29"/>
-      <c r="AF2" s="27"/>
-      <c r="AG2" s="24"/>
-      <c r="AH2" s="24"/>
+      <c r="AC2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD2" s="24"/>
+      <c r="AE2" s="24"/>
+      <c r="AF2" s="24"/>
+      <c r="AG2" s="37"/>
+      <c r="AH2" s="34"/>
+      <c r="AI2" s="34"/>
     </row>
-    <row r="3" spans="1:34" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G3" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="H3" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="H3" s="21" t="s">
-        <v>99</v>
-      </c>
       <c r="I3" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J3" s="21" t="s">
-        <v>18</v>
+        <v>101</v>
       </c>
       <c r="K3" s="21" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="L3" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="M3" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="M3" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="N3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="O3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="21" t="s">
+      <c r="P3" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="20" t="s">
+      <c r="Q3" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="R3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="S3" s="7"/>
-      <c r="T3" s="6" t="s">
+      <c r="T3" s="7"/>
+      <c r="U3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="V3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="W3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="X3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="X3" s="10" t="s">
+      <c r="Y3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="11" t="s">
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="AA3" s="11" t="s">
+      <c r="AB3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="AB3" s="11" t="s">
+      <c r="AC3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="AC3" s="8" t="s">
+      <c r="AD3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="AD3" s="8" t="s">
-        <v>47</v>
-      </c>
       <c r="AE3" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="AF3" s="28"/>
-      <c r="AG3" s="25"/>
-      <c r="AH3" s="25"/>
+        <v>46</v>
+      </c>
+      <c r="AF3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG3" s="38"/>
+      <c r="AH3" s="35"/>
+      <c r="AI3" s="35"/>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>0</v>
       </c>
@@ -1243,10 +1308,10 @@
       <c r="L4" s="4">
         <v>11</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="4">
         <v>12</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="5">
         <v>13</v>
       </c>
       <c r="O4" s="3">
@@ -1261,10 +1326,10 @@
       <c r="R4" s="3">
         <v>17</v>
       </c>
-      <c r="S4" s="5">
+      <c r="S4" s="3">
         <v>18</v>
       </c>
-      <c r="T4" s="3">
+      <c r="T4" s="5">
         <v>19</v>
       </c>
       <c r="U4" s="3">
@@ -1279,10 +1344,10 @@
       <c r="X4" s="3">
         <v>23</v>
       </c>
-      <c r="Y4" s="5">
+      <c r="Y4" s="3">
         <v>24</v>
       </c>
-      <c r="Z4" s="3">
+      <c r="Z4" s="5">
         <v>25</v>
       </c>
       <c r="AA4" s="3">
@@ -1309,359 +1374,580 @@
       <c r="AH4" s="3">
         <v>33</v>
       </c>
+      <c r="AI4" s="3">
+        <v>34</v>
+      </c>
     </row>
-    <row r="5" spans="1:34" ht="48" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" ht="48" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>1</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G5" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="L5" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="K5" s="13" t="s">
+      <c r="M5" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="L5" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="M5" s="14">
+      <c r="N5" s="14">
         <v>30446</v>
       </c>
-      <c r="N5" s="12">
+      <c r="O5" s="12">
         <v>10</v>
       </c>
-      <c r="O5" s="12">
+      <c r="P5" s="12">
         <v>5</v>
       </c>
-      <c r="P5" s="12">
+      <c r="Q5" s="12">
         <v>1983</v>
       </c>
-      <c r="Q5" s="2" t="s">
+      <c r="R5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T5" s="15">
+        <v>39580</v>
+      </c>
+      <c r="U5" s="1">
+        <v>12</v>
+      </c>
+      <c r="V5" s="1">
+        <v>5</v>
+      </c>
+      <c r="W5" s="1">
+        <v>2008</v>
+      </c>
+      <c r="X5" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="R5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="S5" s="15">
-        <v>39580</v>
-      </c>
-      <c r="T5" s="1">
-        <v>12</v>
-      </c>
-      <c r="U5" s="1">
-        <v>5</v>
-      </c>
-      <c r="V5" s="1">
-        <v>2008</v>
-      </c>
-      <c r="W5" s="12" t="s">
+      <c r="Y5" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="X5" s="16" t="s">
+      <c r="Z5" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="Y5" s="15" t="s">
+      <c r="AA5" s="12">
+        <v>25</v>
+      </c>
+      <c r="AB5" s="12">
+        <v>7</v>
+      </c>
+      <c r="AC5" s="12">
+        <v>2003</v>
+      </c>
+      <c r="AD5" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE5" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="Z5" s="12">
-        <v>25</v>
-      </c>
-      <c r="AA5" s="12">
-        <v>7</v>
-      </c>
-      <c r="AB5" s="12">
-        <v>2003</v>
-      </c>
-      <c r="AC5" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD5" s="12" t="s">
+      <c r="AF5" s="12"/>
+      <c r="AG5" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="AE5" s="12"/>
-      <c r="AF5" s="18" t="s">
+      <c r="AH5" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="AG5" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH5" s="17"/>
+      <c r="AI5" s="17"/>
     </row>
-    <row r="6" spans="1:34" ht="48" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" ht="48" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="F6" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="N6" s="14">
+        <v>31619</v>
+      </c>
+      <c r="O6" s="12">
+        <v>26</v>
+      </c>
+      <c r="P6" s="12">
+        <v>7</v>
+      </c>
+      <c r="Q6" s="12">
+        <v>1986</v>
+      </c>
+      <c r="R6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G6" s="12" t="s">
+      <c r="S6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="T6" s="19">
+        <v>40391</v>
+      </c>
+      <c r="U6" s="1">
+        <v>1</v>
+      </c>
+      <c r="V6" s="1">
+        <v>8</v>
+      </c>
+      <c r="W6" s="1">
+        <v>2010</v>
+      </c>
+      <c r="X6" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y6" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z6" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA6" s="12">
+        <v>4</v>
+      </c>
+      <c r="AB6" s="12">
+        <v>3</v>
+      </c>
+      <c r="AC6" s="12">
+        <v>2015</v>
+      </c>
+      <c r="AD6" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE6" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF6" s="12"/>
+      <c r="AG6" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH6" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="AI6" s="18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" ht="48" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="L7" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="H6" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="I6" s="12" t="s">
+      <c r="M7" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="N7" s="14">
+        <v>31620</v>
+      </c>
+      <c r="O7" s="12">
+        <v>27</v>
+      </c>
+      <c r="P7" s="12">
+        <v>7</v>
+      </c>
+      <c r="Q7" s="12">
+        <v>1986</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T7" s="19">
+        <v>40391</v>
+      </c>
+      <c r="U7" s="1">
+        <v>1</v>
+      </c>
+      <c r="V7" s="1">
+        <v>8</v>
+      </c>
+      <c r="W7" s="1">
+        <v>2010</v>
+      </c>
+      <c r="X7" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y7" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z7" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA7" s="12">
+        <v>4</v>
+      </c>
+      <c r="AB7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AC7" s="12">
+        <v>2015</v>
+      </c>
+      <c r="AD7" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE7" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="AF7" s="12"/>
+      <c r="AG7" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="AH7" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="AI7" s="18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" ht="48" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>4</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I8" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="J6" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="K6" s="13" t="s">
+      <c r="J8" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M8" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="L6" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="M6" s="14">
-        <v>31619</v>
-      </c>
-      <c r="N6" s="12">
-        <v>26</v>
-      </c>
-      <c r="O6" s="12">
+      <c r="N8" s="14">
+        <v>31620</v>
+      </c>
+      <c r="O8" s="12">
+        <v>27</v>
+      </c>
+      <c r="P8" s="12">
         <v>7</v>
       </c>
-      <c r="P6" s="12">
+      <c r="Q8" s="12">
         <v>1986</v>
       </c>
-      <c r="Q6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S6" s="19">
+      <c r="R8" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T8" s="19">
         <v>40391</v>
       </c>
-      <c r="T6" s="1">
+      <c r="U8" s="1">
         <v>1</v>
       </c>
-      <c r="U6" s="1">
+      <c r="V8" s="1">
         <v>8</v>
       </c>
-      <c r="V6" s="1">
+      <c r="W8" s="1">
         <v>2010</v>
       </c>
-      <c r="W6" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="X6" s="16" t="s">
+      <c r="X8" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y8" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z8" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="Y6" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z6" s="12">
+      <c r="AA8" s="12">
         <v>4</v>
       </c>
-      <c r="AA6" s="12">
+      <c r="AB8" s="12">
         <v>3</v>
       </c>
-      <c r="AB6" s="12">
+      <c r="AC8" s="12">
         <v>2015</v>
       </c>
-      <c r="AC6" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="AD6" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="AE6" s="12"/>
-      <c r="AF6" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="AG6" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="AH6" s="18" t="s">
-        <v>62</v>
+      <c r="AD8" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE8" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="AF8" s="12"/>
+      <c r="AG8" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="AH8" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="AI8" s="18" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="48" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>2</v>
-      </c>
-      <c r="B7" s="12" t="s">
+    <row r="9" spans="1:35" ht="63.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>5</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="D9" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="E7" s="12" t="s">
+      <c r="E9" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="F7" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="J7" s="13" t="s">
+      <c r="H9" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="N9" s="14">
+        <v>31620</v>
+      </c>
+      <c r="O9" s="12">
+        <v>27</v>
+      </c>
+      <c r="P9" s="12">
+        <v>7</v>
+      </c>
+      <c r="Q9" s="12">
+        <v>1986</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T9" s="19">
+        <v>40391</v>
+      </c>
+      <c r="U9" s="1">
+        <v>1</v>
+      </c>
+      <c r="V9" s="1">
+        <v>8</v>
+      </c>
+      <c r="W9" s="1">
+        <v>2010</v>
+      </c>
+      <c r="X9" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="K7" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="M7" s="14">
-        <v>31620</v>
-      </c>
-      <c r="N7" s="12">
-        <v>27</v>
-      </c>
-      <c r="O7" s="12">
-        <v>7</v>
-      </c>
-      <c r="P7" s="12">
-        <v>1986</v>
-      </c>
-      <c r="Q7" s="2" t="s">
+      <c r="Y9" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="R7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="S7" s="19">
-        <v>40391</v>
-      </c>
-      <c r="T7" s="1">
-        <v>1</v>
-      </c>
-      <c r="U7" s="1">
-        <v>8</v>
-      </c>
-      <c r="V7" s="1">
-        <v>2010</v>
-      </c>
-      <c r="W7" s="12" t="s">
+      <c r="Z9" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA9" s="12">
+        <v>4</v>
+      </c>
+      <c r="AB9" s="12">
+        <v>3</v>
+      </c>
+      <c r="AC9" s="12">
+        <v>2015</v>
+      </c>
+      <c r="AD9" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="X7" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y7" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z7" s="12">
-        <v>4</v>
-      </c>
-      <c r="AA7" s="12">
-        <v>3</v>
-      </c>
-      <c r="AB7" s="12">
-        <v>2015</v>
-      </c>
-      <c r="AC7" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AD7" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="AE7" s="12"/>
-      <c r="AF7" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="AG7" s="12" t="s">
+      <c r="AE9" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="AH7" s="18" t="s">
-        <v>62</v>
+      <c r="AF9" s="12"/>
+      <c r="AG9" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="AH9" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI9" s="18" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-    </row>
-    <row r="10" spans="1:34" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:35" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="R1:R2"/>
+  <mergeCells count="26">
+    <mergeCell ref="AI1:AI3"/>
+    <mergeCell ref="AH1:AH3"/>
+    <mergeCell ref="AG1:AG3"/>
+    <mergeCell ref="AF1:AF2"/>
+    <mergeCell ref="AE1:AE2"/>
+    <mergeCell ref="T1:W1"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="AD1:AD2"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="S1:S2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="M1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="N1:Q2"/>
+    <mergeCell ref="R1:R2"/>
     <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="AC1:AC2"/>
-    <mergeCell ref="Y1:AB1"/>
-    <mergeCell ref="AH1:AH3"/>
-    <mergeCell ref="AG1:AG3"/>
-    <mergeCell ref="AF1:AF3"/>
-    <mergeCell ref="AE1:AE2"/>
-    <mergeCell ref="AD1:AD2"/>
+    <mergeCell ref="K1:K2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="AF6" r:id="rId1" xr:uid="{17D5EC32-5C46-AD47-9FB5-52F61289063A}"/>
-    <hyperlink ref="AF5" r:id="rId2" xr:uid="{7FC0A234-CA60-5049-8E36-12DA086286D9}"/>
-    <hyperlink ref="AF7" r:id="rId3" xr:uid="{11841F35-A7C4-4374-B571-4371FB9F9042}"/>
-    <hyperlink ref="AH6" r:id="rId4" xr:uid="{6A597F78-6AE2-4047-8608-302DE6000859}"/>
-    <hyperlink ref="AH7" r:id="rId5" xr:uid="{E13CBC06-8837-4264-8BC0-3D2BFC682668}"/>
+    <hyperlink ref="AG6" r:id="rId1" xr:uid="{17D5EC32-5C46-AD47-9FB5-52F61289063A}"/>
+    <hyperlink ref="AG5" r:id="rId2" xr:uid="{7FC0A234-CA60-5049-8E36-12DA086286D9}"/>
+    <hyperlink ref="AG7" r:id="rId3" xr:uid="{11841F35-A7C4-4374-B571-4371FB9F9042}"/>
+    <hyperlink ref="AI6" r:id="rId4" xr:uid="{6A597F78-6AE2-4047-8608-302DE6000859}"/>
+    <hyperlink ref="AI7" r:id="rId5" xr:uid="{E13CBC06-8837-4264-8BC0-3D2BFC682668}"/>
+    <hyperlink ref="AG8" r:id="rId6" xr:uid="{5D6A5CCF-6468-440E-90A8-6310F2590E03}"/>
+    <hyperlink ref="AI8" r:id="rId7" xr:uid="{3ABF76DA-623C-4372-87AB-2CF6927AECC4}"/>
+    <hyperlink ref="AG9" r:id="rId8" xr:uid="{3D6A5C86-5A18-49FE-931E-F4B0754DF328}"/>
+    <hyperlink ref="AI9" r:id="rId9" xr:uid="{30E8DCD9-F8BC-4170-9E8B-FBC2E07AC583}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>